<commit_message>
fist commit in new version
</commit_message>
<xml_diff>
--- a/data/yangsan_river.xlsx
+++ b/data/yangsan_river.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\playground\sub_daily_etp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\playground\sub_daily_etp\new_api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2A2278-072D-4D48-9117-BD5D4BBB9234}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0C88C9-CB19-4AF8-92DC-71E7602933AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47FFE701-48A9-4C7F-A49E-9B1CEEFFDE55}"/>
+    <workbookView xWindow="-28485" yWindow="2775" windowWidth="21600" windowHeight="11385" xr2:uid="{47FFE701-48A9-4C7F-A49E-9B1CEEFFDE55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,7 @@
   <dimension ref="A1:K2923"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -484,10 +484,10 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>

</xml_diff>